<commit_message>
Add .csv data files
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RTI\2020\104 3 ฐาน เข้า opendata\datadic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\thai_traffic_deaths\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750F5C96-7822-44C3-9C50-4534DF16C619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E35ECA1-2D3F-44A0-B1F1-770B922E0CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3bura_data_dictionary " sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>อายุผู้เสียชีวิต</t>
   </si>
   <si>
-    <t>เพศผู้เสียชีวิต</t>
-  </si>
-  <si>
     <t>level1 เปิดเผยเฉพาะปีเกิด</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>คำอธิบาย</t>
+  </si>
+  <si>
+    <t>เพศผู้เสียชีวิต 1=ชาย 2=หญิง</t>
   </si>
 </sst>
 </file>
@@ -678,48 +678,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - ส่วนที่ถูกเน้น1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="การคำนวณ" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="ข้อความเตือน" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="ข้อความอธิบาย" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="ชื่อเรื่อง" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="เซลล์ตรวจสอบ" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="เซลล์ที่มีลิงก์" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="ดี" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
-    <cellStyle name="ป้อนค่า" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="ปานกลาง" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="ผลรวม" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="แย่" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="แสดงผล" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="หมายเหตุ" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -735,7 +735,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1034,33 +1034,33 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1114,10 +1114,10 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1125,10 +1125,10 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1136,10 +1136,10 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1147,10 +1147,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1158,10 +1158,10 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1169,10 +1169,10 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1180,10 +1180,10 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1191,10 +1191,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1202,10 +1202,10 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1213,10 +1213,10 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1224,10 +1224,10 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1235,10 +1235,10 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1246,10 +1246,10 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1257,10 +1257,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1268,10 +1268,10 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1279,10 +1279,10 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1290,10 +1290,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1301,10 +1301,10 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1312,10 +1312,10 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1323,10 +1323,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1334,12 +1334,12 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>